<commit_message>
ajustes en filtro de visualizacion y titulo
</commit_message>
<xml_diff>
--- a/results_history/results_15m.xlsx
+++ b/results_history/results_15m.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6289,6 +6289,1098 @@
         </is>
       </c>
     </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:30:04</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2024-05-17 16:45:04</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2024-05-17 17:00:04</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update app.py to show results
</commit_message>
<xml_diff>
--- a/results_history/results_15m.xlsx
+++ b/results_history/results_15m.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F222"/>
+  <dimension ref="A1:F342"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7381,6 +7381,3366 @@
       </c>
       <c r="F222" t="inlineStr"/>
     </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:21:17</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:14</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr"/>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:15</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr"/>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:37:15</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr"/>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2024-05-22 14:52:31</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:07:55</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:23:15</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>SPY</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>BABA</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>DOCN</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>VOO</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>STRONG_BUY</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2024-05-22 15:38:39</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>